<commit_message>
commit refactor code v2
</commit_message>
<xml_diff>
--- a/src/main/resources/config.xlsx
+++ b/src/main/resources/config.xlsx
@@ -484,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D17"/>
+  <dimension ref="B1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,7 +655,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>